<commit_message>
add some values for statistics
</commit_message>
<xml_diff>
--- a/statistics.xlsx
+++ b/statistics.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\WorkSpace\ICT-Project3\ICT-Project3.git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9ABEA85-38D0-457E-A80E-3A0AFD541630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DDD0F9-E872-4923-AAB5-662B9FD047E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9072" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="old result" sheetId="1" r:id="rId1"/>
-    <sheet name="new" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="new" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Iterations</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -65,6 +66,24 @@
   </si>
   <si>
     <t>Mean Similarity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000
+（993）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>6134
+（2099）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ECEM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boundary</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -121,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -129,6 +148,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -136,7 +170,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -156,7 +190,22 @@
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -443,7 +492,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C5" sqref="C5:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -557,11 +606,112 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BBF4FC8-EA91-4563-B094-BE3D44F876AE}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="9">
+        <v>1000</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9">
+        <v>10000</v>
+      </c>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>25</v>
+      </c>
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12">
+        <v>0.60729999999999995</v>
+      </c>
+      <c r="D3" s="11">
+        <v>1</v>
+      </c>
+      <c r="E3" s="12">
+        <v>0.60399999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>50</v>
+      </c>
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.50249999999999995</v>
+      </c>
+      <c r="D4" s="11">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0.50670000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>75</v>
+      </c>
+      <c r="B5" s="11">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.33229999999999998</v>
+      </c>
+      <c r="D5" s="11">
+        <v>1</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.32550000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AC4851-F4F8-4FA1-84D1-71CB9CBD1B51}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -570,11 +720,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -587,7 +737,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>100</v>
       </c>
@@ -598,9 +748,9 @@
         <v>0.97810006317742904</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>1000</v>
+    <row r="4" spans="1:3" ht="34.799999999999997" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="B4" s="6">
         <v>0.91884803380281599</v>
@@ -609,7 +759,17 @@
         <v>0.98557921399606796</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" ht="34.799999999999997" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.84321304498043503</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.99410114633316105</v>
+      </c>
+    </row>
     <row r="6" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">

</xml_diff>